<commit_message>
update examples to reflect reality for tts and stt
</commit_message>
<xml_diff>
--- a/pense/tts/examples/leaderboard/tts_leaderboard.xlsx
+++ b/pense/tts/examples/leaderboard/tts_leaderboard.xlsx
@@ -9,9 +9,7 @@
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="elevenlabs" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="google" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="openai" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="smallest" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="openai" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,73 +469,35 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6463783740997314</v>
+        <v>0.6742491722106934</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0004204114278157552</v>
+        <v>0.0001864433288574219</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>google</t>
+          <t>openai</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3370569944381714</v>
+        <v>1.198368310928345</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7884170532226562</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>openai</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1.528035362561544</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1.958792805671692</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>smallest</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>5</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2.318848371505737</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.0004311005274454753</v>
+        <v>1.634687542915344</v>
       </c>
     </row>
   </sheetData>
@@ -551,7 +511,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -562,42 +522,14 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>text</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>audio_path</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>llm_judge_score</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>llm_judge_reasoning</t>
+          <t>info</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>And your full address—could you tell me your village, block, and district?</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>/Users/aman/Documents/repos/artpark/agentloop/data/basic/human/english/tts_output/elevenlabs/audios/2.wav</t>
-        </is>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>The reference text is: 'And your full address—could you tell me your village, block, and district?' The audio says: 'And your full address, could you tell me your village, block, and districts?' The audio is almost identical to the reference text, except for the pluralization of 'district' to 'districts' in the audio. This is a minor difference, but it does slightly alter the text. Overall, the text is easily understandable from the audio, with only a small deviation.</t>
+          <t>No results.csv found</t>
         </is>
       </c>
     </row>
@@ -637,70 +569,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>info</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>No results.csv found</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>info</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>No results.csv found</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
cleanup both tts and stt to not use pipecat
</commit_message>
<xml_diff>
--- a/pense/tts/examples/leaderboard/tts_leaderboard.xlsx
+++ b/pense/tts/examples/leaderboard/tts_leaderboard.xlsx
@@ -475,11 +475,9 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6742491722106934</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.0001864433288574219</v>
-      </c>
+        <v>1.362950086593628</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -494,11 +492,9 @@
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>1.198368310928345</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1.634687542915344</v>
-      </c>
+        <v>1.769400477409363</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>